<commit_message>
modification upload for tracker
</commit_message>
<xml_diff>
--- a/Test_tracker.xlsx
+++ b/Test_tracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\mygitstudy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\mygitstudy\MyGitStudy101\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,8 +479,12 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>

</xml_diff>